<commit_message>
updates to espn_fantasy_scrap and init Jan27 notebook
</commit_message>
<xml_diff>
--- a/autvinc_table.xlsx
+++ b/autvinc_table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="31">
   <si>
     <t>Delonte's Donuts</t>
   </si>
@@ -177,7 +177,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -219,17 +219,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -269,6 +275,14 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -599,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N461"/>
+  <dimension ref="A1:M511"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A429" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B463" sqref="B463"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A477" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D515" sqref="D515"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14595,7 +14609,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="369" spans="1:13">
+    <row r="369" spans="1:12">
       <c r="A369" s="1" t="s">
         <v>9</v>
       </c>
@@ -14633,7 +14647,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="370" spans="1:13">
+    <row r="370" spans="1:12">
       <c r="A370" s="1" t="s">
         <v>7</v>
       </c>
@@ -14671,7 +14685,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="371" spans="1:13">
+    <row r="371" spans="1:12">
       <c r="A371" s="1" t="s">
         <v>5</v>
       </c>
@@ -14709,7 +14723,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="372" spans="1:13">
+    <row r="372" spans="1:12">
       <c r="A372" s="1" t="s">
         <v>0</v>
       </c>
@@ -14746,9 +14760,8 @@
       <c r="L372" s="3">
         <v>562</v>
       </c>
-      <c r="M372" s="2"/>
-    </row>
-    <row r="373" spans="1:13">
+    </row>
+    <row r="373" spans="1:12">
       <c r="A373" s="1" t="s">
         <v>1</v>
       </c>
@@ -14785,9 +14798,8 @@
       <c r="L373" s="2">
         <v>402</v>
       </c>
-      <c r="M373" s="2"/>
-    </row>
-    <row r="374" spans="1:13">
+    </row>
+    <row r="374" spans="1:12">
       <c r="A374" s="1" t="s">
         <v>24</v>
       </c>
@@ -14824,9 +14836,8 @@
       <c r="L374" s="2">
         <v>559</v>
       </c>
-      <c r="M374" s="2"/>
-    </row>
-    <row r="375" spans="1:13">
+    </row>
+    <row r="375" spans="1:12">
       <c r="A375" s="1" t="s">
         <v>28</v>
       </c>
@@ -14863,9 +14874,8 @@
       <c r="L375" s="2">
         <v>559</v>
       </c>
-      <c r="M375" s="2"/>
-    </row>
-    <row r="376" spans="1:13">
+    </row>
+    <row r="376" spans="1:12">
       <c r="A376" s="1" t="s">
         <v>29</v>
       </c>
@@ -14902,9 +14912,8 @@
       <c r="L376" s="3">
         <v>561</v>
       </c>
-      <c r="M376" s="2"/>
-    </row>
-    <row r="377" spans="1:13">
+    </row>
+    <row r="377" spans="1:12">
       <c r="A377" s="1" t="s">
         <v>30</v>
       </c>
@@ -14941,9 +14950,8 @@
       <c r="L377" s="2">
         <v>434</v>
       </c>
-      <c r="M377" s="2"/>
-    </row>
-    <row r="378" spans="1:13">
+    </row>
+    <row r="378" spans="1:12">
       <c r="A378" s="1" t="s">
         <v>6</v>
       </c>
@@ -14980,9 +14988,8 @@
       <c r="L378" s="2">
         <v>469</v>
       </c>
-      <c r="M378" s="2"/>
-    </row>
-    <row r="379" spans="1:13">
+    </row>
+    <row r="379" spans="1:12">
       <c r="A379" s="1" t="s">
         <v>7</v>
       </c>
@@ -15019,9 +15026,8 @@
       <c r="L379" s="3">
         <v>532</v>
       </c>
-      <c r="M379" s="2"/>
-    </row>
-    <row r="380" spans="1:13">
+    </row>
+    <row r="380" spans="1:12">
       <c r="A380" s="1" t="s">
         <v>26</v>
       </c>
@@ -15058,9 +15064,8 @@
       <c r="L380" s="3">
         <v>549</v>
       </c>
-      <c r="M380" s="2"/>
-    </row>
-    <row r="381" spans="1:13">
+    </row>
+    <row r="381" spans="1:12">
       <c r="A381" s="1" t="s">
         <v>9</v>
       </c>
@@ -15097,9 +15102,8 @@
       <c r="L381" s="2">
         <v>530</v>
       </c>
-      <c r="M381" s="2"/>
-    </row>
-    <row r="382" spans="1:13">
+    </row>
+    <row r="382" spans="1:12">
       <c r="A382" s="1" t="s">
         <v>0</v>
       </c>
@@ -15136,9 +15140,8 @@
       <c r="L382" s="2">
         <v>651</v>
       </c>
-      <c r="M382" s="2"/>
-    </row>
-    <row r="383" spans="1:13">
+    </row>
+    <row r="383" spans="1:12">
       <c r="A383" s="1" t="s">
         <v>26</v>
       </c>
@@ -15175,9 +15178,8 @@
       <c r="L383" s="3">
         <v>744</v>
       </c>
-      <c r="M383" s="2"/>
-    </row>
-    <row r="384" spans="1:13">
+    </row>
+    <row r="384" spans="1:12">
       <c r="A384" s="1" t="s">
         <v>29</v>
       </c>
@@ -15214,9 +15216,8 @@
       <c r="L384" s="3">
         <v>659</v>
       </c>
-      <c r="M384" s="2"/>
-    </row>
-    <row r="385" spans="1:13">
+    </row>
+    <row r="385" spans="1:12">
       <c r="A385" s="1" t="s">
         <v>24</v>
       </c>
@@ -15253,9 +15254,8 @@
       <c r="L385" s="2">
         <v>503</v>
       </c>
-      <c r="M385" s="2"/>
-    </row>
-    <row r="386" spans="1:13">
+    </row>
+    <row r="386" spans="1:12">
       <c r="A386" s="1" t="s">
         <v>1</v>
       </c>
@@ -15292,9 +15292,8 @@
       <c r="L386" s="2">
         <v>572</v>
       </c>
-      <c r="M386" s="2"/>
-    </row>
-    <row r="387" spans="1:13">
+    </row>
+    <row r="387" spans="1:12">
       <c r="A387" s="1" t="s">
         <v>6</v>
       </c>
@@ -15331,9 +15330,8 @@
       <c r="L387" s="3">
         <v>605</v>
       </c>
-      <c r="M387" s="2"/>
-    </row>
-    <row r="388" spans="1:13">
+    </row>
+    <row r="388" spans="1:12">
       <c r="A388" s="1" t="s">
         <v>28</v>
       </c>
@@ -15370,9 +15368,8 @@
       <c r="L388" s="2">
         <v>688</v>
       </c>
-      <c r="M388" s="2"/>
-    </row>
-    <row r="389" spans="1:13">
+    </row>
+    <row r="389" spans="1:12">
       <c r="A389" s="1" t="s">
         <v>7</v>
       </c>
@@ -15409,9 +15406,8 @@
       <c r="L389" s="3">
         <v>741</v>
       </c>
-      <c r="M389" s="2"/>
-    </row>
-    <row r="390" spans="1:13">
+    </row>
+    <row r="390" spans="1:12">
       <c r="A390" s="1" t="s">
         <v>30</v>
       </c>
@@ -15448,9 +15444,8 @@
       <c r="L390" s="2">
         <v>529</v>
       </c>
-      <c r="M390" s="2"/>
-    </row>
-    <row r="391" spans="1:13">
+    </row>
+    <row r="391" spans="1:12">
       <c r="A391" s="1" t="s">
         <v>9</v>
       </c>
@@ -15487,9 +15482,8 @@
       <c r="L391" s="3">
         <v>619</v>
       </c>
-      <c r="M391" s="2"/>
-    </row>
-    <row r="392" spans="1:13">
+    </row>
+    <row r="392" spans="1:12">
       <c r="A392" s="1" t="s">
         <v>30</v>
       </c>
@@ -15526,9 +15520,8 @@
       <c r="L392" s="2">
         <v>642</v>
       </c>
-      <c r="M392" s="2"/>
-    </row>
-    <row r="393" spans="1:13">
+    </row>
+    <row r="393" spans="1:12">
       <c r="A393" s="1" t="s">
         <v>0</v>
       </c>
@@ -15565,9 +15558,8 @@
       <c r="L393" s="3">
         <v>777</v>
       </c>
-      <c r="M393" s="2"/>
-    </row>
-    <row r="394" spans="1:13">
+    </row>
+    <row r="394" spans="1:12">
       <c r="A394" s="1" t="s">
         <v>26</v>
       </c>
@@ -15604,9 +15596,8 @@
       <c r="L394" s="3">
         <v>808</v>
       </c>
-      <c r="M394" s="2"/>
-    </row>
-    <row r="395" spans="1:13">
+    </row>
+    <row r="395" spans="1:12">
       <c r="A395" s="1" t="s">
         <v>27</v>
       </c>
@@ -15643,9 +15634,8 @@
       <c r="L395" s="2">
         <v>728</v>
       </c>
-      <c r="M395" s="2"/>
-    </row>
-    <row r="396" spans="1:13">
+    </row>
+    <row r="396" spans="1:12">
       <c r="A396" s="1" t="s">
         <v>7</v>
       </c>
@@ -15682,9 +15672,8 @@
       <c r="L396" s="3">
         <v>736</v>
       </c>
-      <c r="M396" s="2"/>
-    </row>
-    <row r="397" spans="1:13">
+    </row>
+    <row r="397" spans="1:12">
       <c r="A397" s="1" t="s">
         <v>24</v>
       </c>
@@ -15721,9 +15710,8 @@
       <c r="L397" s="2">
         <v>596</v>
       </c>
-      <c r="M397" s="2"/>
-    </row>
-    <row r="398" spans="1:13">
+    </row>
+    <row r="398" spans="1:12">
       <c r="A398" s="1" t="s">
         <v>9</v>
       </c>
@@ -15760,9 +15748,8 @@
       <c r="L398" s="2">
         <v>597</v>
       </c>
-      <c r="M398" s="2"/>
-    </row>
-    <row r="399" spans="1:13">
+    </row>
+    <row r="399" spans="1:12">
       <c r="A399" s="1" t="s">
         <v>29</v>
       </c>
@@ -15799,9 +15786,8 @@
       <c r="L399" s="3">
         <v>690</v>
       </c>
-      <c r="M399" s="2"/>
-    </row>
-    <row r="400" spans="1:13">
+    </row>
+    <row r="400" spans="1:12">
       <c r="A400" s="1" t="s">
         <v>28</v>
       </c>
@@ -15838,9 +15824,8 @@
       <c r="L400" s="3">
         <v>637</v>
       </c>
-      <c r="M400" s="2"/>
-    </row>
-    <row r="401" spans="1:13">
+    </row>
+    <row r="401" spans="1:12">
       <c r="A401" s="1" t="s">
         <v>1</v>
       </c>
@@ -15877,9 +15862,8 @@
       <c r="L401" s="2">
         <v>504</v>
       </c>
-      <c r="M401" s="2"/>
-    </row>
-    <row r="402" spans="1:13">
+    </row>
+    <row r="402" spans="1:12">
       <c r="A402" s="1" t="s">
         <v>29</v>
       </c>
@@ -15916,9 +15900,8 @@
       <c r="L402" s="2">
         <v>633</v>
       </c>
-      <c r="M402" s="2"/>
-    </row>
-    <row r="403" spans="1:13">
+    </row>
+    <row r="403" spans="1:12">
       <c r="A403" s="1" t="s">
         <v>0</v>
       </c>
@@ -15955,9 +15938,8 @@
       <c r="L403" s="3">
         <v>703</v>
       </c>
-      <c r="M403" s="2"/>
-    </row>
-    <row r="404" spans="1:13">
+    </row>
+    <row r="404" spans="1:12">
       <c r="A404" s="1" t="s">
         <v>9</v>
       </c>
@@ -15994,9 +15976,8 @@
       <c r="L404" s="2">
         <v>557</v>
       </c>
-      <c r="M404" s="2"/>
-    </row>
-    <row r="405" spans="1:13">
+    </row>
+    <row r="405" spans="1:12">
       <c r="A405" s="1" t="s">
         <v>7</v>
       </c>
@@ -16033,9 +16014,8 @@
       <c r="L405" s="3">
         <v>753</v>
       </c>
-      <c r="M405" s="2"/>
-    </row>
-    <row r="406" spans="1:13">
+    </row>
+    <row r="406" spans="1:12">
       <c r="A406" s="1" t="s">
         <v>6</v>
       </c>
@@ -16072,9 +16052,8 @@
       <c r="L406" s="2">
         <v>660</v>
       </c>
-      <c r="M406" s="2"/>
-    </row>
-    <row r="407" spans="1:13">
+    </row>
+    <row r="407" spans="1:12">
       <c r="A407" s="1" t="s">
         <v>28</v>
       </c>
@@ -16111,9 +16090,8 @@
       <c r="L407" s="3">
         <v>813</v>
       </c>
-      <c r="M407" s="2"/>
-    </row>
-    <row r="408" spans="1:13">
+    </row>
+    <row r="408" spans="1:12">
       <c r="A408" s="1" t="s">
         <v>26</v>
       </c>
@@ -16150,9 +16128,8 @@
       <c r="L408" s="3">
         <v>651</v>
       </c>
-      <c r="M408" s="2"/>
-    </row>
-    <row r="409" spans="1:13">
+    </row>
+    <row r="409" spans="1:12">
       <c r="A409" s="1" t="s">
         <v>30</v>
       </c>
@@ -16189,9 +16166,8 @@
       <c r="L409" s="2">
         <v>622</v>
       </c>
-      <c r="M409" s="2"/>
-    </row>
-    <row r="410" spans="1:13">
+    </row>
+    <row r="410" spans="1:12">
       <c r="A410" s="1" t="s">
         <v>24</v>
       </c>
@@ -16228,9 +16204,8 @@
       <c r="L410" s="2">
         <v>473</v>
       </c>
-      <c r="M410" s="2"/>
-    </row>
-    <row r="411" spans="1:13">
+    </row>
+    <row r="411" spans="1:12">
       <c r="A411" s="1" t="s">
         <v>1</v>
       </c>
@@ -16267,9 +16242,8 @@
       <c r="L411" s="3">
         <v>598</v>
       </c>
-      <c r="M411" s="2"/>
-    </row>
-    <row r="412" spans="1:13">
+    </row>
+    <row r="412" spans="1:12">
       <c r="A412" s="1" t="s">
         <v>0</v>
       </c>
@@ -16306,9 +16280,8 @@
       <c r="L412" s="2">
         <v>645</v>
       </c>
-      <c r="M412" s="2"/>
-    </row>
-    <row r="413" spans="1:13">
+    </row>
+    <row r="413" spans="1:12">
       <c r="A413" s="1" t="s">
         <v>9</v>
       </c>
@@ -16345,9 +16318,8 @@
       <c r="L413" s="3">
         <v>725</v>
       </c>
-      <c r="M413" s="2"/>
-    </row>
-    <row r="414" spans="1:13">
+    </row>
+    <row r="414" spans="1:12">
       <c r="A414" s="1" t="s">
         <v>30</v>
       </c>
@@ -16384,9 +16356,8 @@
       <c r="L414" s="2">
         <v>631</v>
       </c>
-      <c r="M414" s="2"/>
-    </row>
-    <row r="415" spans="1:13">
+    </row>
+    <row r="415" spans="1:12">
       <c r="A415" s="1" t="s">
         <v>28</v>
       </c>
@@ -16423,9 +16394,8 @@
       <c r="L415" s="3">
         <v>713</v>
       </c>
-      <c r="M415" s="2"/>
-    </row>
-    <row r="416" spans="1:13">
+    </row>
+    <row r="416" spans="1:12">
       <c r="A416" s="1" t="s">
         <v>1</v>
       </c>
@@ -16462,9 +16432,8 @@
       <c r="L416" s="2">
         <v>561</v>
       </c>
-      <c r="M416" s="2"/>
-    </row>
-    <row r="417" spans="1:14">
+    </row>
+    <row r="417" spans="1:12">
       <c r="A417" s="1" t="s">
         <v>7</v>
       </c>
@@ -16501,9 +16470,8 @@
       <c r="L417" s="3">
         <v>697</v>
       </c>
-      <c r="M417" s="2"/>
-    </row>
-    <row r="418" spans="1:14">
+    </row>
+    <row r="418" spans="1:12">
       <c r="A418" s="1" t="s">
         <v>24</v>
       </c>
@@ -16540,9 +16508,8 @@
       <c r="L418" s="2">
         <v>612</v>
       </c>
-      <c r="M418" s="2"/>
-    </row>
-    <row r="419" spans="1:14">
+    </row>
+    <row r="419" spans="1:12">
       <c r="A419" s="1" t="s">
         <v>6</v>
       </c>
@@ -16579,9 +16546,8 @@
       <c r="L419" s="3">
         <v>644</v>
       </c>
-      <c r="M419" s="2"/>
-    </row>
-    <row r="420" spans="1:14">
+    </row>
+    <row r="420" spans="1:12">
       <c r="A420" s="1" t="s">
         <v>29</v>
       </c>
@@ -16618,9 +16584,8 @@
       <c r="L420" s="2">
         <v>661</v>
       </c>
-      <c r="M420" s="2"/>
-    </row>
-    <row r="421" spans="1:14">
+    </row>
+    <row r="421" spans="1:12">
       <c r="A421" s="1" t="s">
         <v>26</v>
       </c>
@@ -16657,9 +16622,8 @@
       <c r="L421" s="3">
         <v>685</v>
       </c>
-      <c r="M421" s="2"/>
-    </row>
-    <row r="422" spans="1:14">
+    </row>
+    <row r="422" spans="1:12">
       <c r="A422" s="1" t="s">
         <v>24</v>
       </c>
@@ -16696,9 +16660,8 @@
       <c r="L422" s="3">
         <v>664</v>
       </c>
-      <c r="M422" s="2"/>
-    </row>
-    <row r="423" spans="1:14">
+    </row>
+    <row r="423" spans="1:12">
       <c r="A423" s="1" t="s">
         <v>0</v>
       </c>
@@ -16735,9 +16698,8 @@
       <c r="L423" s="2">
         <v>625</v>
       </c>
-      <c r="M423" s="2"/>
-    </row>
-    <row r="424" spans="1:14">
+    </row>
+    <row r="424" spans="1:12">
       <c r="A424" s="1" t="s">
         <v>6</v>
       </c>
@@ -16774,9 +16736,8 @@
       <c r="L424" s="3">
         <v>588</v>
       </c>
-      <c r="M424" s="2"/>
-    </row>
-    <row r="425" spans="1:14">
+    </row>
+    <row r="425" spans="1:12">
       <c r="A425" s="1" t="s">
         <v>29</v>
       </c>
@@ -16813,9 +16774,8 @@
       <c r="L425" s="2">
         <v>522</v>
       </c>
-      <c r="M425" s="2"/>
-    </row>
-    <row r="426" spans="1:14">
+    </row>
+    <row r="426" spans="1:12">
       <c r="A426" s="1" t="s">
         <v>7</v>
       </c>
@@ -16852,9 +16812,8 @@
       <c r="L426" s="3">
         <v>744</v>
       </c>
-      <c r="M426" s="2"/>
-    </row>
-    <row r="427" spans="1:14">
+    </row>
+    <row r="427" spans="1:12">
       <c r="A427" s="1" t="s">
         <v>26</v>
       </c>
@@ -16891,9 +16850,8 @@
       <c r="L427" s="2">
         <v>678</v>
       </c>
-      <c r="M427" s="2"/>
-    </row>
-    <row r="428" spans="1:14">
+    </row>
+    <row r="428" spans="1:12">
       <c r="A428" s="1" t="s">
         <v>28</v>
       </c>
@@ -16930,9 +16888,8 @@
       <c r="L428" s="2">
         <v>685</v>
       </c>
-      <c r="M428" s="2"/>
-    </row>
-    <row r="429" spans="1:14">
+    </row>
+    <row r="429" spans="1:12">
       <c r="A429" s="1" t="s">
         <v>9</v>
       </c>
@@ -16969,9 +16926,8 @@
       <c r="L429" s="3">
         <v>696</v>
       </c>
-      <c r="M429" s="2"/>
-    </row>
-    <row r="430" spans="1:14">
+    </row>
+    <row r="430" spans="1:12">
       <c r="A430" s="1" t="s">
         <v>1</v>
       </c>
@@ -17008,9 +16964,8 @@
       <c r="L430" s="2">
         <v>571</v>
       </c>
-      <c r="M430" s="2"/>
-    </row>
-    <row r="431" spans="1:14">
+    </row>
+    <row r="431" spans="1:12">
       <c r="A431" s="1" t="s">
         <v>30</v>
       </c>
@@ -17047,9 +17002,8 @@
       <c r="L431" s="3">
         <v>611</v>
       </c>
-      <c r="M431" s="2"/>
-    </row>
-    <row r="432" spans="1:14">
+    </row>
+    <row r="432" spans="1:12">
       <c r="A432" s="1" t="s">
         <v>0</v>
       </c>
@@ -17086,10 +17040,8 @@
       <c r="L432" s="2">
         <v>688</v>
       </c>
-      <c r="M432" s="2"/>
-      <c r="N432" s="5"/>
-    </row>
-    <row r="433" spans="1:14">
+    </row>
+    <row r="433" spans="1:12">
       <c r="A433" s="1" t="s">
         <v>6</v>
       </c>
@@ -17126,10 +17078,8 @@
       <c r="L433" s="3">
         <v>820</v>
       </c>
-      <c r="M433" s="2"/>
-      <c r="N433" s="6"/>
-    </row>
-    <row r="434" spans="1:14">
+    </row>
+    <row r="434" spans="1:12">
       <c r="A434" s="1" t="s">
         <v>29</v>
       </c>
@@ -17166,10 +17116,8 @@
       <c r="L434" s="3">
         <v>722</v>
       </c>
-      <c r="M434" s="2"/>
-      <c r="N434" s="5"/>
-    </row>
-    <row r="435" spans="1:14">
+    </row>
+    <row r="435" spans="1:12">
       <c r="A435" s="1" t="s">
         <v>7</v>
       </c>
@@ -17206,10 +17154,8 @@
       <c r="L435" s="2">
         <v>708</v>
       </c>
-      <c r="M435" s="2"/>
-      <c r="N435" s="6"/>
-    </row>
-    <row r="436" spans="1:14">
+    </row>
+    <row r="436" spans="1:12">
       <c r="A436" s="1" t="s">
         <v>26</v>
       </c>
@@ -17246,10 +17192,8 @@
       <c r="L436" s="3">
         <v>920</v>
       </c>
-      <c r="M436" s="2"/>
-      <c r="N436" s="5"/>
-    </row>
-    <row r="437" spans="1:14">
+    </row>
+    <row r="437" spans="1:12">
       <c r="A437" s="1" t="s">
         <v>28</v>
       </c>
@@ -17286,10 +17230,8 @@
       <c r="L437" s="2">
         <v>562</v>
       </c>
-      <c r="M437" s="2"/>
-      <c r="N437" s="6"/>
-    </row>
-    <row r="438" spans="1:14">
+    </row>
+    <row r="438" spans="1:12">
       <c r="A438" s="1" t="s">
         <v>9</v>
       </c>
@@ -17326,10 +17268,8 @@
       <c r="L438" s="3">
         <v>852</v>
       </c>
-      <c r="M438" s="2"/>
-      <c r="N438" s="5"/>
-    </row>
-    <row r="439" spans="1:14">
+    </row>
+    <row r="439" spans="1:12">
       <c r="A439" s="1" t="s">
         <v>1</v>
       </c>
@@ -17366,10 +17306,8 @@
       <c r="L439" s="2">
         <v>709</v>
       </c>
-      <c r="M439" s="2"/>
-      <c r="N439" s="6"/>
-    </row>
-    <row r="440" spans="1:14">
+    </row>
+    <row r="440" spans="1:12">
       <c r="A440" s="1" t="s">
         <v>30</v>
       </c>
@@ -17406,10 +17344,8 @@
       <c r="L440" s="3">
         <v>702</v>
       </c>
-      <c r="M440" s="2"/>
-      <c r="N440" s="5"/>
-    </row>
-    <row r="441" spans="1:14">
+    </row>
+    <row r="441" spans="1:12">
       <c r="A441" s="1" t="s">
         <v>24</v>
       </c>
@@ -17446,10 +17382,8 @@
       <c r="L441" s="2">
         <v>660</v>
       </c>
-      <c r="M441" s="2"/>
-      <c r="N441" s="6"/>
-    </row>
-    <row r="442" spans="1:14">
+    </row>
+    <row r="442" spans="1:12">
       <c r="A442" s="1" t="s">
         <v>7</v>
       </c>
@@ -17486,10 +17420,8 @@
       <c r="L442" s="3">
         <v>699</v>
       </c>
-      <c r="M442" s="2"/>
-      <c r="N442" s="6"/>
-    </row>
-    <row r="443" spans="1:14">
+    </row>
+    <row r="443" spans="1:12">
       <c r="A443" s="1" t="s">
         <v>0</v>
       </c>
@@ -17526,10 +17458,8 @@
       <c r="L443" s="2">
         <v>666</v>
       </c>
-      <c r="M443" s="2"/>
-      <c r="N443" s="5"/>
-    </row>
-    <row r="444" spans="1:14">
+    </row>
+    <row r="444" spans="1:12">
       <c r="A444" s="1" t="s">
         <v>28</v>
       </c>
@@ -17566,10 +17496,8 @@
       <c r="L444" s="3">
         <v>667</v>
       </c>
-      <c r="M444" s="2"/>
-      <c r="N444" s="6"/>
-    </row>
-    <row r="445" spans="1:14">
+    </row>
+    <row r="445" spans="1:12">
       <c r="A445" s="1" t="s">
         <v>29</v>
       </c>
@@ -17606,10 +17534,8 @@
       <c r="L445" s="2">
         <v>631</v>
       </c>
-      <c r="M445" s="2"/>
-      <c r="N445" s="5"/>
-    </row>
-    <row r="446" spans="1:14">
+    </row>
+    <row r="446" spans="1:12">
       <c r="A446" s="1" t="s">
         <v>1</v>
       </c>
@@ -17646,10 +17572,8 @@
       <c r="L446" s="2">
         <v>592</v>
       </c>
-      <c r="M446" s="2"/>
-      <c r="N446" s="5"/>
-    </row>
-    <row r="447" spans="1:14">
+    </row>
+    <row r="447" spans="1:12">
       <c r="A447" s="1" t="s">
         <v>26</v>
       </c>
@@ -17686,10 +17610,8 @@
       <c r="L447" s="3">
         <v>611</v>
       </c>
-      <c r="M447" s="2"/>
-      <c r="N447" s="6"/>
-    </row>
-    <row r="448" spans="1:14">
+    </row>
+    <row r="448" spans="1:12">
       <c r="A448" s="1" t="s">
         <v>24</v>
       </c>
@@ -17726,10 +17648,8 @@
       <c r="L448" s="2">
         <v>646</v>
       </c>
-      <c r="M448" s="2"/>
-      <c r="N448" s="6"/>
-    </row>
-    <row r="449" spans="1:14">
+    </row>
+    <row r="449" spans="1:12">
       <c r="A449" s="1" t="s">
         <v>9</v>
       </c>
@@ -17766,10 +17686,8 @@
       <c r="L449" s="3">
         <v>734</v>
       </c>
-      <c r="M449" s="2"/>
-      <c r="N449" s="5"/>
-    </row>
-    <row r="450" spans="1:14">
+    </row>
+    <row r="450" spans="1:12">
       <c r="A450" s="1" t="s">
         <v>6</v>
       </c>
@@ -17806,10 +17724,8 @@
       <c r="L450" s="3">
         <v>654</v>
       </c>
-      <c r="M450" s="2"/>
-      <c r="N450" s="6"/>
-    </row>
-    <row r="451" spans="1:14">
+    </row>
+    <row r="451" spans="1:12">
       <c r="A451" s="1" t="s">
         <v>30</v>
       </c>
@@ -17846,10 +17762,8 @@
       <c r="L451" s="2">
         <v>574</v>
       </c>
-      <c r="M451" s="2"/>
-      <c r="N451" s="6"/>
-    </row>
-    <row r="452" spans="1:14">
+    </row>
+    <row r="452" spans="1:12">
       <c r="A452" s="1" t="s">
         <v>0</v>
       </c>
@@ -17886,10 +17800,8 @@
       <c r="L452" s="2">
         <v>603</v>
       </c>
-      <c r="M452" s="2"/>
-      <c r="N452" s="5"/>
-    </row>
-    <row r="453" spans="1:14">
+    </row>
+    <row r="453" spans="1:12">
       <c r="A453" s="1" t="s">
         <v>28</v>
       </c>
@@ -17926,10 +17838,8 @@
       <c r="L453" s="3">
         <v>676</v>
       </c>
-      <c r="M453" s="2"/>
-      <c r="N453" s="6"/>
-    </row>
-    <row r="454" spans="1:14">
+    </row>
+    <row r="454" spans="1:12">
       <c r="A454" s="1" t="s">
         <v>7</v>
       </c>
@@ -17966,10 +17876,8 @@
       <c r="L454" s="2">
         <v>493</v>
       </c>
-      <c r="M454" s="2"/>
-      <c r="N454" s="6"/>
-    </row>
-    <row r="455" spans="1:14">
+    </row>
+    <row r="455" spans="1:12">
       <c r="A455" s="1" t="s">
         <v>1</v>
       </c>
@@ -18006,10 +17914,8 @@
       <c r="L455" s="3">
         <v>594</v>
       </c>
-      <c r="M455" s="2"/>
-      <c r="N455" s="5"/>
-    </row>
-    <row r="456" spans="1:14">
+    </row>
+    <row r="456" spans="1:12">
       <c r="A456" s="1" t="s">
         <v>30</v>
       </c>
@@ -18046,10 +17952,8 @@
       <c r="L456" s="2">
         <v>656</v>
       </c>
-      <c r="M456" s="2"/>
-      <c r="N456" s="5"/>
-    </row>
-    <row r="457" spans="1:14">
+    </row>
+    <row r="457" spans="1:12">
       <c r="A457" s="1" t="s">
         <v>29</v>
       </c>
@@ -18086,10 +17990,8 @@
       <c r="L457" s="3">
         <v>671</v>
       </c>
-      <c r="M457" s="2"/>
-      <c r="N457" s="6"/>
-    </row>
-    <row r="458" spans="1:14">
+    </row>
+    <row r="458" spans="1:12">
       <c r="A458" s="1" t="s">
         <v>6</v>
       </c>
@@ -18126,10 +18028,8 @@
       <c r="L458" s="2">
         <v>614</v>
       </c>
-      <c r="M458" s="2"/>
-      <c r="N458" s="6"/>
-    </row>
-    <row r="459" spans="1:14">
+    </row>
+    <row r="459" spans="1:12">
       <c r="A459" s="1" t="s">
         <v>24</v>
       </c>
@@ -18166,10 +18066,8 @@
       <c r="L459" s="3">
         <v>671</v>
       </c>
-      <c r="M459" s="2"/>
-      <c r="N459" s="5"/>
-    </row>
-    <row r="460" spans="1:14">
+    </row>
+    <row r="460" spans="1:12">
       <c r="A460" s="1" t="s">
         <v>9</v>
       </c>
@@ -18206,10 +18104,8 @@
       <c r="L460" s="3">
         <v>673</v>
       </c>
-      <c r="M460" s="2"/>
-      <c r="N460" s="5"/>
-    </row>
-    <row r="461" spans="1:14">
+    </row>
+    <row r="461" spans="1:12">
       <c r="A461" s="1" t="s">
         <v>26</v>
       </c>
@@ -18246,8 +18142,1916 @@
       <c r="L461" s="2">
         <v>621</v>
       </c>
-      <c r="M461" s="2"/>
-      <c r="N461" s="6"/>
+    </row>
+    <row r="462" spans="1:12">
+      <c r="A462" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B462" s="2">
+        <v>10</v>
+      </c>
+      <c r="C462" s="2">
+        <v>3</v>
+      </c>
+      <c r="D462" s="2">
+        <v>0.436</v>
+      </c>
+      <c r="E462" s="3">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="F462" s="3">
+        <v>62</v>
+      </c>
+      <c r="G462" s="2">
+        <v>188</v>
+      </c>
+      <c r="H462" s="3">
+        <v>144</v>
+      </c>
+      <c r="I462" s="3">
+        <v>41</v>
+      </c>
+      <c r="J462" s="2">
+        <v>10</v>
+      </c>
+      <c r="K462" s="3">
+        <v>61</v>
+      </c>
+      <c r="L462" s="2">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="463" spans="1:12">
+      <c r="A463" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B463" s="2">
+        <v>10</v>
+      </c>
+      <c r="C463" s="2">
+        <v>3</v>
+      </c>
+      <c r="D463" s="3">
+        <v>0.52310000000000001</v>
+      </c>
+      <c r="E463" s="2">
+        <v>0.78569999999999995</v>
+      </c>
+      <c r="F463" s="2">
+        <v>60</v>
+      </c>
+      <c r="G463" s="3">
+        <v>240</v>
+      </c>
+      <c r="H463" s="2">
+        <v>119</v>
+      </c>
+      <c r="I463" s="2">
+        <v>32</v>
+      </c>
+      <c r="J463" s="3">
+        <v>40</v>
+      </c>
+      <c r="K463" s="2">
+        <v>77</v>
+      </c>
+      <c r="L463" s="3">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="464" spans="1:12">
+      <c r="A464" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B464" s="2">
+        <v>10</v>
+      </c>
+      <c r="C464" s="2">
+        <v>3</v>
+      </c>
+      <c r="D464" s="2">
+        <v>0.44119999999999998</v>
+      </c>
+      <c r="E464" s="3">
+        <v>0.81459999999999999</v>
+      </c>
+      <c r="F464" s="3">
+        <v>50</v>
+      </c>
+      <c r="G464" s="3">
+        <v>307</v>
+      </c>
+      <c r="H464" s="3">
+        <v>181</v>
+      </c>
+      <c r="I464" s="3">
+        <v>50</v>
+      </c>
+      <c r="J464" s="3">
+        <v>31</v>
+      </c>
+      <c r="K464" s="2">
+        <v>108</v>
+      </c>
+      <c r="L464" s="3">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="465" spans="1:12">
+      <c r="A465" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B465" s="2">
+        <v>10</v>
+      </c>
+      <c r="C465" s="2">
+        <v>3</v>
+      </c>
+      <c r="D465" s="3">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="E465" s="2">
+        <v>0.79069999999999996</v>
+      </c>
+      <c r="F465" s="2">
+        <v>49</v>
+      </c>
+      <c r="G465" s="2">
+        <v>259</v>
+      </c>
+      <c r="H465" s="2">
+        <v>139</v>
+      </c>
+      <c r="I465" s="2">
+        <v>42</v>
+      </c>
+      <c r="J465" s="2">
+        <v>20</v>
+      </c>
+      <c r="K465" s="3">
+        <v>69</v>
+      </c>
+      <c r="L465" s="2">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="466" spans="1:12">
+      <c r="A466" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B466" s="2">
+        <v>10</v>
+      </c>
+      <c r="C466" s="2">
+        <v>3</v>
+      </c>
+      <c r="D466" s="3">
+        <v>0.46650000000000003</v>
+      </c>
+      <c r="E466" s="3">
+        <v>0.87839999999999996</v>
+      </c>
+      <c r="F466" s="3">
+        <v>58</v>
+      </c>
+      <c r="G466" s="2">
+        <v>198</v>
+      </c>
+      <c r="H466" s="3">
+        <v>150</v>
+      </c>
+      <c r="I466" s="2">
+        <v>41</v>
+      </c>
+      <c r="J466" s="3">
+        <v>24</v>
+      </c>
+      <c r="K466" s="2">
+        <v>94</v>
+      </c>
+      <c r="L466" s="3">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="467" spans="1:12">
+      <c r="A467" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B467" s="2">
+        <v>10</v>
+      </c>
+      <c r="C467" s="2">
+        <v>3</v>
+      </c>
+      <c r="D467" s="2">
+        <v>0.45989999999999998</v>
+      </c>
+      <c r="E467" s="2">
+        <v>0.7883</v>
+      </c>
+      <c r="F467" s="2">
+        <v>50</v>
+      </c>
+      <c r="G467" s="3">
+        <v>227</v>
+      </c>
+      <c r="H467" s="2">
+        <v>130</v>
+      </c>
+      <c r="I467" s="2">
+        <v>41</v>
+      </c>
+      <c r="J467" s="2">
+        <v>17</v>
+      </c>
+      <c r="K467" s="2">
+        <v>94</v>
+      </c>
+      <c r="L467" s="2">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="468" spans="1:12">
+      <c r="A468" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B468" s="2">
+        <v>10</v>
+      </c>
+      <c r="C468" s="2">
+        <v>3</v>
+      </c>
+      <c r="D468" s="2">
+        <v>0.45590000000000003</v>
+      </c>
+      <c r="E468" s="3">
+        <v>0.77349999999999997</v>
+      </c>
+      <c r="F468" s="2">
+        <v>26</v>
+      </c>
+      <c r="G468" s="3">
+        <v>264</v>
+      </c>
+      <c r="H468" s="2">
+        <v>134</v>
+      </c>
+      <c r="I468" s="2">
+        <v>43</v>
+      </c>
+      <c r="J468" s="3">
+        <v>25</v>
+      </c>
+      <c r="K468" s="3">
+        <v>87</v>
+      </c>
+      <c r="L468" s="2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="469" spans="1:12">
+      <c r="A469" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B469" s="2">
+        <v>10</v>
+      </c>
+      <c r="C469" s="2">
+        <v>3</v>
+      </c>
+      <c r="D469" s="3">
+        <v>0.49220000000000003</v>
+      </c>
+      <c r="E469" s="2">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="F469" s="3">
+        <v>74</v>
+      </c>
+      <c r="G469" s="2">
+        <v>216</v>
+      </c>
+      <c r="H469" s="3">
+        <v>164</v>
+      </c>
+      <c r="I469" s="3">
+        <v>50</v>
+      </c>
+      <c r="J469" s="2">
+        <v>17</v>
+      </c>
+      <c r="K469" s="2">
+        <v>91</v>
+      </c>
+      <c r="L469" s="3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="470" spans="1:12">
+      <c r="A470" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B470" s="2">
+        <v>10</v>
+      </c>
+      <c r="C470" s="2">
+        <v>3</v>
+      </c>
+      <c r="D470" s="2">
+        <v>0.48420000000000002</v>
+      </c>
+      <c r="E470" s="3">
+        <v>0.78220000000000001</v>
+      </c>
+      <c r="F470" s="3">
+        <v>54</v>
+      </c>
+      <c r="G470" s="2">
+        <v>209</v>
+      </c>
+      <c r="H470" s="2">
+        <v>115</v>
+      </c>
+      <c r="I470" s="2">
+        <v>37</v>
+      </c>
+      <c r="J470" s="3">
+        <v>28</v>
+      </c>
+      <c r="K470" s="3">
+        <v>57</v>
+      </c>
+      <c r="L470" s="3">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="471" spans="1:12">
+      <c r="A471" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B471" s="2">
+        <v>10</v>
+      </c>
+      <c r="C471" s="2">
+        <v>3</v>
+      </c>
+      <c r="D471" s="3">
+        <v>0.48880000000000001</v>
+      </c>
+      <c r="E471" s="2">
+        <v>0.76419999999999999</v>
+      </c>
+      <c r="F471" s="2">
+        <v>39</v>
+      </c>
+      <c r="G471" s="3">
+        <v>229</v>
+      </c>
+      <c r="H471" s="3">
+        <v>129</v>
+      </c>
+      <c r="I471" s="3">
+        <v>42</v>
+      </c>
+      <c r="J471" s="2">
+        <v>23</v>
+      </c>
+      <c r="K471" s="2">
+        <v>66</v>
+      </c>
+      <c r="L471" s="2">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="472" spans="1:12">
+      <c r="A472" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B472" s="2">
+        <v>11</v>
+      </c>
+      <c r="C472" s="2">
+        <v>3</v>
+      </c>
+      <c r="D472" s="2">
+        <v>0.46239999999999998</v>
+      </c>
+      <c r="E472" s="3">
+        <v>0.79549999999999998</v>
+      </c>
+      <c r="F472" s="2">
+        <v>62</v>
+      </c>
+      <c r="G472" s="3">
+        <v>289</v>
+      </c>
+      <c r="H472" s="2">
+        <v>167</v>
+      </c>
+      <c r="I472" s="2">
+        <v>49</v>
+      </c>
+      <c r="J472" s="3">
+        <v>63</v>
+      </c>
+      <c r="K472" s="3">
+        <v>84</v>
+      </c>
+      <c r="L472" s="2">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="473" spans="1:12">
+      <c r="A473" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B473" s="2">
+        <v>11</v>
+      </c>
+      <c r="C473" s="2">
+        <v>3</v>
+      </c>
+      <c r="D473" s="3">
+        <v>0.48309999999999997</v>
+      </c>
+      <c r="E473" s="2">
+        <v>0.73819999999999997</v>
+      </c>
+      <c r="F473" s="3">
+        <v>63</v>
+      </c>
+      <c r="G473" s="2">
+        <v>285</v>
+      </c>
+      <c r="H473" s="3">
+        <v>170</v>
+      </c>
+      <c r="I473" s="3">
+        <v>52</v>
+      </c>
+      <c r="J473" s="2">
+        <v>26</v>
+      </c>
+      <c r="K473" s="2">
+        <v>93</v>
+      </c>
+      <c r="L473" s="2">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="474" spans="1:12">
+      <c r="A474" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B474" s="2">
+        <v>11</v>
+      </c>
+      <c r="C474" s="2">
+        <v>3</v>
+      </c>
+      <c r="D474" s="3">
+        <v>0.46360000000000001</v>
+      </c>
+      <c r="E474" s="2">
+        <v>0.74070000000000003</v>
+      </c>
+      <c r="F474" s="2">
+        <v>71</v>
+      </c>
+      <c r="G474" s="2">
+        <v>265</v>
+      </c>
+      <c r="H474" s="3">
+        <v>185</v>
+      </c>
+      <c r="I474" s="3">
+        <v>49</v>
+      </c>
+      <c r="J474" s="2">
+        <v>23</v>
+      </c>
+      <c r="K474" s="3">
+        <v>98</v>
+      </c>
+      <c r="L474" s="3">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="475" spans="1:12">
+      <c r="A475" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B475" s="2">
+        <v>11</v>
+      </c>
+      <c r="C475" s="2">
+        <v>3</v>
+      </c>
+      <c r="D475" s="2">
+        <v>0.44109999999999999</v>
+      </c>
+      <c r="E475" s="3">
+        <v>0.84150000000000003</v>
+      </c>
+      <c r="F475" s="3">
+        <v>82</v>
+      </c>
+      <c r="G475" s="3">
+        <v>274</v>
+      </c>
+      <c r="H475" s="2">
+        <v>151</v>
+      </c>
+      <c r="I475" s="2">
+        <v>35</v>
+      </c>
+      <c r="J475" s="3">
+        <v>32</v>
+      </c>
+      <c r="K475" s="2">
+        <v>102</v>
+      </c>
+      <c r="L475" s="2">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="476" spans="1:12">
+      <c r="A476" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B476" s="2">
+        <v>11</v>
+      </c>
+      <c r="C476" s="2">
+        <v>3</v>
+      </c>
+      <c r="D476" s="2">
+        <v>0.4637</v>
+      </c>
+      <c r="E476" s="3">
+        <v>0.7964</v>
+      </c>
+      <c r="F476" s="2">
+        <v>56</v>
+      </c>
+      <c r="G476" s="2">
+        <v>214</v>
+      </c>
+      <c r="H476" s="3">
+        <v>166</v>
+      </c>
+      <c r="I476" s="3">
+        <v>56</v>
+      </c>
+      <c r="J476" s="2">
+        <v>21</v>
+      </c>
+      <c r="K476" s="2">
+        <v>93</v>
+      </c>
+      <c r="L476" s="3">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="477" spans="1:12">
+      <c r="A477" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B477" s="2">
+        <v>11</v>
+      </c>
+      <c r="C477" s="2">
+        <v>3</v>
+      </c>
+      <c r="D477" s="3">
+        <v>0.47320000000000001</v>
+      </c>
+      <c r="E477" s="2">
+        <v>0.76129999999999998</v>
+      </c>
+      <c r="F477" s="3">
+        <v>59</v>
+      </c>
+      <c r="G477" s="3">
+        <v>270</v>
+      </c>
+      <c r="H477" s="2">
+        <v>144</v>
+      </c>
+      <c r="I477" s="2">
+        <v>30</v>
+      </c>
+      <c r="J477" s="3">
+        <v>31</v>
+      </c>
+      <c r="K477" s="3">
+        <v>57</v>
+      </c>
+      <c r="L477" s="2">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="478" spans="1:12">
+      <c r="A478" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B478" s="2">
+        <v>11</v>
+      </c>
+      <c r="C478" s="2">
+        <v>3</v>
+      </c>
+      <c r="D478" s="2">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="E478" s="3">
+        <v>0.84470000000000001</v>
+      </c>
+      <c r="F478" s="2">
+        <v>38</v>
+      </c>
+      <c r="G478" s="3">
+        <v>324</v>
+      </c>
+      <c r="H478" s="3">
+        <v>166</v>
+      </c>
+      <c r="I478" s="2">
+        <v>50</v>
+      </c>
+      <c r="J478" s="3">
+        <v>38</v>
+      </c>
+      <c r="K478" s="2">
+        <v>109</v>
+      </c>
+      <c r="L478" s="2">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="479" spans="1:12">
+      <c r="A479" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B479" s="2">
+        <v>11</v>
+      </c>
+      <c r="C479" s="2">
+        <v>3</v>
+      </c>
+      <c r="D479" s="3">
+        <v>0.49020000000000002</v>
+      </c>
+      <c r="E479" s="2">
+        <v>0.83620000000000005</v>
+      </c>
+      <c r="F479" s="3">
+        <v>58</v>
+      </c>
+      <c r="G479" s="2">
+        <v>275</v>
+      </c>
+      <c r="H479" s="2">
+        <v>121</v>
+      </c>
+      <c r="I479" s="3">
+        <v>51</v>
+      </c>
+      <c r="J479" s="2">
+        <v>15</v>
+      </c>
+      <c r="K479" s="3">
+        <v>69</v>
+      </c>
+      <c r="L479" s="3">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="480" spans="1:12">
+      <c r="A480" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B480" s="2">
+        <v>11</v>
+      </c>
+      <c r="C480" s="2">
+        <v>3</v>
+      </c>
+      <c r="D480" s="3">
+        <v>0.45290000000000002</v>
+      </c>
+      <c r="E480" s="2">
+        <v>0.82489999999999997</v>
+      </c>
+      <c r="F480" s="2">
+        <v>59</v>
+      </c>
+      <c r="G480" s="3">
+        <v>252</v>
+      </c>
+      <c r="H480" s="2">
+        <v>112</v>
+      </c>
+      <c r="I480" s="2">
+        <v>29</v>
+      </c>
+      <c r="J480" s="2">
+        <v>21</v>
+      </c>
+      <c r="K480" s="3">
+        <v>70</v>
+      </c>
+      <c r="L480" s="2">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="481" spans="1:12">
+      <c r="A481" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B481" s="2">
+        <v>11</v>
+      </c>
+      <c r="C481" s="2">
+        <v>3</v>
+      </c>
+      <c r="D481" s="2">
+        <v>0.44829999999999998</v>
+      </c>
+      <c r="E481" s="3">
+        <v>0.86519999999999997</v>
+      </c>
+      <c r="F481" s="3">
+        <v>79</v>
+      </c>
+      <c r="G481" s="2">
+        <v>230</v>
+      </c>
+      <c r="H481" s="3">
+        <v>185</v>
+      </c>
+      <c r="I481" s="3">
+        <v>40</v>
+      </c>
+      <c r="J481" s="3">
+        <v>25</v>
+      </c>
+      <c r="K481" s="2">
+        <v>82</v>
+      </c>
+      <c r="L481" s="3">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="482" spans="1:12">
+      <c r="A482" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B482" s="2">
+        <v>12</v>
+      </c>
+      <c r="C482" s="2">
+        <v>3</v>
+      </c>
+      <c r="D482" s="2">
+        <v>0.47149999999999997</v>
+      </c>
+      <c r="E482" s="3">
+        <v>0.85260000000000002</v>
+      </c>
+      <c r="F482" s="2">
+        <v>39</v>
+      </c>
+      <c r="G482" s="2">
+        <v>208</v>
+      </c>
+      <c r="H482" s="2">
+        <v>104</v>
+      </c>
+      <c r="I482" s="3">
+        <v>46</v>
+      </c>
+      <c r="J482" s="3">
+        <v>25</v>
+      </c>
+      <c r="K482" s="3">
+        <v>60</v>
+      </c>
+      <c r="L482" s="2">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="483" spans="1:12">
+      <c r="A483" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B483" s="2">
+        <v>12</v>
+      </c>
+      <c r="C483" s="2">
+        <v>3</v>
+      </c>
+      <c r="D483" s="3">
+        <v>0.48780000000000001</v>
+      </c>
+      <c r="E483" s="2">
+        <v>0.82220000000000004</v>
+      </c>
+      <c r="F483" s="2">
+        <v>39</v>
+      </c>
+      <c r="G483" s="3">
+        <v>251</v>
+      </c>
+      <c r="H483" s="3">
+        <v>123</v>
+      </c>
+      <c r="I483" s="2">
+        <v>28</v>
+      </c>
+      <c r="J483" s="2">
+        <v>21</v>
+      </c>
+      <c r="K483" s="2">
+        <v>80</v>
+      </c>
+      <c r="L483" s="3">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="484" spans="1:12">
+      <c r="A484" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B484" s="2">
+        <v>12</v>
+      </c>
+      <c r="C484" s="2">
+        <v>3</v>
+      </c>
+      <c r="D484" s="2">
+        <v>0.44190000000000002</v>
+      </c>
+      <c r="E484" s="3">
+        <v>0.83520000000000005</v>
+      </c>
+      <c r="F484" s="2">
+        <v>45</v>
+      </c>
+      <c r="G484" s="2">
+        <v>160</v>
+      </c>
+      <c r="H484" s="2">
+        <v>91</v>
+      </c>
+      <c r="I484" s="2">
+        <v>22</v>
+      </c>
+      <c r="J484" s="2">
+        <v>14</v>
+      </c>
+      <c r="K484" s="3">
+        <v>45</v>
+      </c>
+      <c r="L484" s="2">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="485" spans="1:12">
+      <c r="A485" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B485" s="2">
+        <v>12</v>
+      </c>
+      <c r="C485" s="2">
+        <v>3</v>
+      </c>
+      <c r="D485" s="3">
+        <v>0.44519999999999998</v>
+      </c>
+      <c r="E485" s="2">
+        <v>0.65280000000000005</v>
+      </c>
+      <c r="F485" s="3">
+        <v>50</v>
+      </c>
+      <c r="G485" s="3">
+        <v>218</v>
+      </c>
+      <c r="H485" s="3">
+        <v>150</v>
+      </c>
+      <c r="I485" s="3">
+        <v>49</v>
+      </c>
+      <c r="J485" s="3">
+        <v>33</v>
+      </c>
+      <c r="K485" s="2">
+        <v>75</v>
+      </c>
+      <c r="L485" s="3">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="486" spans="1:12">
+      <c r="A486" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B486" s="2">
+        <v>12</v>
+      </c>
+      <c r="C486" s="2">
+        <v>3</v>
+      </c>
+      <c r="D486" s="2">
+        <v>0.46960000000000002</v>
+      </c>
+      <c r="E486" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="F486" s="2">
+        <v>56</v>
+      </c>
+      <c r="G486" s="2">
+        <v>257</v>
+      </c>
+      <c r="H486" s="3">
+        <v>137</v>
+      </c>
+      <c r="I486" s="2">
+        <v>32</v>
+      </c>
+      <c r="J486" s="2">
+        <v>14</v>
+      </c>
+      <c r="K486" s="2">
+        <v>89</v>
+      </c>
+      <c r="L486" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="487" spans="1:12">
+      <c r="A487" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B487" s="2">
+        <v>12</v>
+      </c>
+      <c r="C487" s="2">
+        <v>3</v>
+      </c>
+      <c r="D487" s="3">
+        <v>0.52810000000000001</v>
+      </c>
+      <c r="E487" s="2">
+        <v>0.7349</v>
+      </c>
+      <c r="F487" s="3">
+        <v>63</v>
+      </c>
+      <c r="G487" s="3">
+        <v>270</v>
+      </c>
+      <c r="H487" s="2">
+        <v>119</v>
+      </c>
+      <c r="I487" s="3">
+        <v>36</v>
+      </c>
+      <c r="J487" s="3">
+        <v>34</v>
+      </c>
+      <c r="K487" s="3">
+        <v>76</v>
+      </c>
+      <c r="L487" s="3">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="488" spans="1:12">
+      <c r="A488" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B488" s="2">
+        <v>12</v>
+      </c>
+      <c r="C488" s="2">
+        <v>3</v>
+      </c>
+      <c r="D488" s="3">
+        <v>0.49559999999999998</v>
+      </c>
+      <c r="E488" s="3">
+        <v>0.8054</v>
+      </c>
+      <c r="F488" s="2">
+        <v>49</v>
+      </c>
+      <c r="G488" s="3">
+        <v>241</v>
+      </c>
+      <c r="H488" s="2">
+        <v>106</v>
+      </c>
+      <c r="I488" s="2">
+        <v>35</v>
+      </c>
+      <c r="J488" s="3">
+        <v>26</v>
+      </c>
+      <c r="K488" s="3">
+        <v>66</v>
+      </c>
+      <c r="L488" s="2">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="489" spans="1:12">
+      <c r="A489" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B489" s="2">
+        <v>12</v>
+      </c>
+      <c r="C489" s="2">
+        <v>3</v>
+      </c>
+      <c r="D489" s="2">
+        <v>0.45660000000000001</v>
+      </c>
+      <c r="E489" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="F489" s="3">
+        <v>66</v>
+      </c>
+      <c r="G489" s="2">
+        <v>204</v>
+      </c>
+      <c r="H489" s="3">
+        <v>181</v>
+      </c>
+      <c r="I489" s="3">
+        <v>52</v>
+      </c>
+      <c r="J489" s="2">
+        <v>17</v>
+      </c>
+      <c r="K489" s="2">
+        <v>99</v>
+      </c>
+      <c r="L489" s="3">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="490" spans="1:12">
+      <c r="A490" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B490" s="2">
+        <v>12</v>
+      </c>
+      <c r="C490" s="2">
+        <v>3</v>
+      </c>
+      <c r="D490" s="2">
+        <v>0.46750000000000003</v>
+      </c>
+      <c r="E490" s="2">
+        <v>0.6552</v>
+      </c>
+      <c r="F490" s="2">
+        <v>50</v>
+      </c>
+      <c r="G490" s="3">
+        <v>204</v>
+      </c>
+      <c r="H490" s="2">
+        <v>104</v>
+      </c>
+      <c r="I490" s="2">
+        <v>22</v>
+      </c>
+      <c r="J490" s="2">
+        <v>15</v>
+      </c>
+      <c r="K490" s="3">
+        <v>55</v>
+      </c>
+      <c r="L490" s="2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="491" spans="1:12">
+      <c r="A491" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B491" s="2">
+        <v>12</v>
+      </c>
+      <c r="C491" s="2">
+        <v>3</v>
+      </c>
+      <c r="D491" s="3">
+        <v>0.46929999999999999</v>
+      </c>
+      <c r="E491" s="3">
+        <v>0.76870000000000005</v>
+      </c>
+      <c r="F491" s="3">
+        <v>52</v>
+      </c>
+      <c r="G491" s="2">
+        <v>184</v>
+      </c>
+      <c r="H491" s="3">
+        <v>172</v>
+      </c>
+      <c r="I491" s="3">
+        <v>43</v>
+      </c>
+      <c r="J491" s="3">
+        <v>16</v>
+      </c>
+      <c r="K491" s="2">
+        <v>82</v>
+      </c>
+      <c r="L491" s="3">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="492" spans="1:12">
+      <c r="A492" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B492" s="2">
+        <v>13</v>
+      </c>
+      <c r="C492" s="2">
+        <v>3</v>
+      </c>
+      <c r="D492" s="3">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="E492" s="3">
+        <v>0.81340000000000001</v>
+      </c>
+      <c r="F492" s="2">
+        <v>63</v>
+      </c>
+      <c r="G492" s="2">
+        <v>206</v>
+      </c>
+      <c r="H492" s="2">
+        <v>128</v>
+      </c>
+      <c r="I492" s="2">
+        <v>38</v>
+      </c>
+      <c r="J492" s="2">
+        <v>32</v>
+      </c>
+      <c r="K492" s="3">
+        <v>73</v>
+      </c>
+      <c r="L492" s="2">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="493" spans="1:12">
+      <c r="A493" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B493" s="2">
+        <v>13</v>
+      </c>
+      <c r="C493" s="2">
+        <v>3</v>
+      </c>
+      <c r="D493" s="2">
+        <v>0.50170000000000003</v>
+      </c>
+      <c r="E493" s="2">
+        <v>0.7167</v>
+      </c>
+      <c r="F493" s="3">
+        <v>82</v>
+      </c>
+      <c r="G493" s="3">
+        <v>307</v>
+      </c>
+      <c r="H493" s="3">
+        <v>155</v>
+      </c>
+      <c r="I493" s="3">
+        <v>54</v>
+      </c>
+      <c r="J493" s="3">
+        <v>54</v>
+      </c>
+      <c r="K493" s="2">
+        <v>92</v>
+      </c>
+      <c r="L493" s="3">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="494" spans="1:12">
+      <c r="A494" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B494" s="2">
+        <v>13</v>
+      </c>
+      <c r="C494" s="2">
+        <v>3</v>
+      </c>
+      <c r="D494" s="3">
+        <v>0.47789999999999999</v>
+      </c>
+      <c r="E494" s="2">
+        <v>0.74519999999999997</v>
+      </c>
+      <c r="F494" s="3">
+        <v>47</v>
+      </c>
+      <c r="G494" s="2">
+        <v>231</v>
+      </c>
+      <c r="H494" s="2">
+        <v>140</v>
+      </c>
+      <c r="I494" s="2">
+        <v>36</v>
+      </c>
+      <c r="J494" s="3">
+        <v>35</v>
+      </c>
+      <c r="K494" s="3">
+        <v>81</v>
+      </c>
+      <c r="L494" s="2">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="495" spans="1:12">
+      <c r="A495" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B495" s="2">
+        <v>13</v>
+      </c>
+      <c r="C495" s="2">
+        <v>3</v>
+      </c>
+      <c r="D495" s="2">
+        <v>0.46889999999999998</v>
+      </c>
+      <c r="E495" s="3">
+        <v>0.7833</v>
+      </c>
+      <c r="F495" s="2">
+        <v>37</v>
+      </c>
+      <c r="G495" s="3">
+        <v>264</v>
+      </c>
+      <c r="H495" s="3">
+        <v>152</v>
+      </c>
+      <c r="I495" s="3">
+        <v>47</v>
+      </c>
+      <c r="J495" s="2">
+        <v>24</v>
+      </c>
+      <c r="K495" s="2">
+        <v>92</v>
+      </c>
+      <c r="L495" s="3">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="496" spans="1:12">
+      <c r="A496" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B496" s="2">
+        <v>13</v>
+      </c>
+      <c r="C496" s="2">
+        <v>3</v>
+      </c>
+      <c r="D496" s="3">
+        <v>0.45979999999999999</v>
+      </c>
+      <c r="E496" s="3">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="F496" s="2">
+        <v>62</v>
+      </c>
+      <c r="G496" s="3">
+        <v>218</v>
+      </c>
+      <c r="H496" s="3">
+        <v>160</v>
+      </c>
+      <c r="I496" s="2">
+        <v>33</v>
+      </c>
+      <c r="J496" s="3">
+        <v>23</v>
+      </c>
+      <c r="K496" s="3">
+        <v>90</v>
+      </c>
+      <c r="L496" s="3">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="497" spans="1:13">
+      <c r="A497" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B497" s="2">
+        <v>13</v>
+      </c>
+      <c r="C497" s="2">
+        <v>3</v>
+      </c>
+      <c r="D497" s="2">
+        <v>0.42549999999999999</v>
+      </c>
+      <c r="E497" s="2">
+        <v>0.77710000000000001</v>
+      </c>
+      <c r="F497" s="2">
+        <v>62</v>
+      </c>
+      <c r="G497" s="2">
+        <v>197</v>
+      </c>
+      <c r="H497" s="2">
+        <v>149</v>
+      </c>
+      <c r="I497" s="3">
+        <v>67</v>
+      </c>
+      <c r="J497" s="2">
+        <v>16</v>
+      </c>
+      <c r="K497" s="2">
+        <v>95</v>
+      </c>
+      <c r="L497" s="2">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="498" spans="1:13">
+      <c r="A498" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B498" s="2">
+        <v>13</v>
+      </c>
+      <c r="C498" s="2">
+        <v>3</v>
+      </c>
+      <c r="D498" s="3">
+        <v>0.4733</v>
+      </c>
+      <c r="E498" s="2">
+        <v>0.79490000000000005</v>
+      </c>
+      <c r="F498" s="2">
+        <v>41</v>
+      </c>
+      <c r="G498" s="2">
+        <v>200</v>
+      </c>
+      <c r="H498" s="2">
+        <v>124</v>
+      </c>
+      <c r="I498" s="2">
+        <v>23</v>
+      </c>
+      <c r="J498" s="2">
+        <v>19</v>
+      </c>
+      <c r="K498" s="3">
+        <v>71</v>
+      </c>
+      <c r="L498" s="2">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="499" spans="1:13">
+      <c r="A499" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B499" s="2">
+        <v>13</v>
+      </c>
+      <c r="C499" s="2">
+        <v>3</v>
+      </c>
+      <c r="D499" s="2">
+        <v>0.4244</v>
+      </c>
+      <c r="E499" s="3">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="F499" s="3">
+        <v>58</v>
+      </c>
+      <c r="G499" s="3">
+        <v>251</v>
+      </c>
+      <c r="H499" s="3">
+        <v>135</v>
+      </c>
+      <c r="I499" s="3">
+        <v>37</v>
+      </c>
+      <c r="J499" s="3">
+        <v>25</v>
+      </c>
+      <c r="K499" s="2">
+        <v>73</v>
+      </c>
+      <c r="L499" s="3">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="500" spans="1:13">
+      <c r="A500" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B500" s="2">
+        <v>13</v>
+      </c>
+      <c r="C500" s="2">
+        <v>3</v>
+      </c>
+      <c r="D500" s="2">
+        <v>0.44440000000000002</v>
+      </c>
+      <c r="E500" s="2">
+        <v>0.80920000000000003</v>
+      </c>
+      <c r="F500" s="3">
+        <v>75</v>
+      </c>
+      <c r="G500" s="2">
+        <v>230</v>
+      </c>
+      <c r="H500" s="3">
+        <v>167</v>
+      </c>
+      <c r="I500" s="3">
+        <v>38</v>
+      </c>
+      <c r="J500" s="2">
+        <v>24</v>
+      </c>
+      <c r="K500" s="2">
+        <v>99</v>
+      </c>
+      <c r="L500" s="2">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="501" spans="1:13">
+      <c r="A501" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B501" s="2">
+        <v>13</v>
+      </c>
+      <c r="C501" s="2">
+        <v>3</v>
+      </c>
+      <c r="D501" s="3">
+        <v>0.49349999999999999</v>
+      </c>
+      <c r="E501" s="3">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="F501" s="2">
+        <v>36</v>
+      </c>
+      <c r="G501" s="3">
+        <v>247</v>
+      </c>
+      <c r="H501" s="2">
+        <v>157</v>
+      </c>
+      <c r="I501" s="2">
+        <v>37</v>
+      </c>
+      <c r="J501" s="3">
+        <v>25</v>
+      </c>
+      <c r="K501" s="3">
+        <v>82</v>
+      </c>
+      <c r="L501" s="3">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="502" spans="1:13">
+      <c r="A502" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B502" s="2">
+        <v>14</v>
+      </c>
+      <c r="C502" s="2">
+        <v>3</v>
+      </c>
+      <c r="D502" s="2">
+        <v>0.44929999999999998</v>
+      </c>
+      <c r="E502" s="3">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="F502" s="2">
+        <v>39</v>
+      </c>
+      <c r="G502" s="2">
+        <v>267</v>
+      </c>
+      <c r="H502" s="2">
+        <v>146</v>
+      </c>
+      <c r="I502" s="2">
+        <v>31</v>
+      </c>
+      <c r="J502" s="2">
+        <v>26</v>
+      </c>
+      <c r="K502" s="2">
+        <v>95</v>
+      </c>
+      <c r="L502" s="2">
+        <v>660</v>
+      </c>
+      <c r="M502" s="2"/>
+    </row>
+    <row r="503" spans="1:13">
+      <c r="A503" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B503" s="2">
+        <v>14</v>
+      </c>
+      <c r="C503" s="2">
+        <v>3</v>
+      </c>
+      <c r="D503" s="3">
+        <v>0.48720000000000002</v>
+      </c>
+      <c r="E503" s="2">
+        <v>0.80920000000000003</v>
+      </c>
+      <c r="F503" s="3">
+        <v>62</v>
+      </c>
+      <c r="G503" s="3">
+        <v>271</v>
+      </c>
+      <c r="H503" s="3">
+        <v>180</v>
+      </c>
+      <c r="I503" s="3">
+        <v>46</v>
+      </c>
+      <c r="J503" s="3">
+        <v>51</v>
+      </c>
+      <c r="K503" s="3">
+        <v>83</v>
+      </c>
+      <c r="L503" s="3">
+        <v>774</v>
+      </c>
+      <c r="M503" s="2"/>
+    </row>
+    <row r="504" spans="1:13">
+      <c r="A504" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B504" s="2">
+        <v>14</v>
+      </c>
+      <c r="C504" s="2">
+        <v>3</v>
+      </c>
+      <c r="D504" s="2">
+        <v>0.43140000000000001</v>
+      </c>
+      <c r="E504" s="3">
+        <v>0.83740000000000003</v>
+      </c>
+      <c r="F504" s="3">
+        <v>69</v>
+      </c>
+      <c r="G504" s="2">
+        <v>283</v>
+      </c>
+      <c r="H504" s="3">
+        <v>171</v>
+      </c>
+      <c r="I504" s="2">
+        <v>55</v>
+      </c>
+      <c r="J504" s="2">
+        <v>23</v>
+      </c>
+      <c r="K504" s="3">
+        <v>93</v>
+      </c>
+      <c r="L504" s="2">
+        <v>755</v>
+      </c>
+      <c r="M504" s="2"/>
+    </row>
+    <row r="505" spans="1:13">
+      <c r="A505" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B505" s="2">
+        <v>14</v>
+      </c>
+      <c r="C505" s="2">
+        <v>3</v>
+      </c>
+      <c r="D505" s="3">
+        <v>0.4894</v>
+      </c>
+      <c r="E505" s="2">
+        <v>0.80289999999999995</v>
+      </c>
+      <c r="F505" s="2">
+        <v>44</v>
+      </c>
+      <c r="G505" s="3">
+        <v>356</v>
+      </c>
+      <c r="H505" s="2">
+        <v>170</v>
+      </c>
+      <c r="I505" s="3">
+        <v>59</v>
+      </c>
+      <c r="J505" s="3">
+        <v>41</v>
+      </c>
+      <c r="K505" s="2">
+        <v>123</v>
+      </c>
+      <c r="L505" s="3">
+        <v>763</v>
+      </c>
+      <c r="M505" s="2"/>
+    </row>
+    <row r="506" spans="1:13">
+      <c r="A506" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B506" s="2">
+        <v>14</v>
+      </c>
+      <c r="C506" s="2">
+        <v>3</v>
+      </c>
+      <c r="D506" s="3">
+        <v>0.49580000000000002</v>
+      </c>
+      <c r="E506" s="2">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="F506" s="3">
+        <v>69</v>
+      </c>
+      <c r="G506" s="2">
+        <v>191</v>
+      </c>
+      <c r="H506" s="3">
+        <v>170</v>
+      </c>
+      <c r="I506" s="3">
+        <v>47</v>
+      </c>
+      <c r="J506" s="3">
+        <v>19</v>
+      </c>
+      <c r="K506" s="2">
+        <v>94</v>
+      </c>
+      <c r="L506" s="3">
+        <v>811</v>
+      </c>
+      <c r="M506" s="2"/>
+    </row>
+    <row r="507" spans="1:13">
+      <c r="A507" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B507" s="2">
+        <v>14</v>
+      </c>
+      <c r="C507" s="2">
+        <v>3</v>
+      </c>
+      <c r="D507" s="2">
+        <v>0.4829</v>
+      </c>
+      <c r="E507" s="3">
+        <v>0.79620000000000002</v>
+      </c>
+      <c r="F507" s="2">
+        <v>61</v>
+      </c>
+      <c r="G507" s="3">
+        <v>210</v>
+      </c>
+      <c r="H507" s="2">
+        <v>145</v>
+      </c>
+      <c r="I507" s="2">
+        <v>36</v>
+      </c>
+      <c r="J507" s="2">
+        <v>17</v>
+      </c>
+      <c r="K507" s="3">
+        <v>78</v>
+      </c>
+      <c r="L507" s="2">
+        <v>722</v>
+      </c>
+      <c r="M507" s="2"/>
+    </row>
+    <row r="508" spans="1:13">
+      <c r="A508" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B508" s="2">
+        <v>14</v>
+      </c>
+      <c r="C508" s="2">
+        <v>3</v>
+      </c>
+      <c r="D508" s="2">
+        <v>0.49419999999999997</v>
+      </c>
+      <c r="E508" s="2">
+        <v>0.75660000000000005</v>
+      </c>
+      <c r="F508" s="2">
+        <v>47</v>
+      </c>
+      <c r="G508" s="3">
+        <v>239</v>
+      </c>
+      <c r="H508" s="2">
+        <v>103</v>
+      </c>
+      <c r="I508" s="2">
+        <v>39</v>
+      </c>
+      <c r="J508" s="2">
+        <v>22</v>
+      </c>
+      <c r="K508" s="3">
+        <v>68</v>
+      </c>
+      <c r="L508" s="2">
+        <v>670</v>
+      </c>
+      <c r="M508" s="2"/>
+    </row>
+    <row r="509" spans="1:13">
+      <c r="A509" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B509" s="2">
+        <v>14</v>
+      </c>
+      <c r="C509" s="2">
+        <v>3</v>
+      </c>
+      <c r="D509" s="3">
+        <v>0.50280000000000002</v>
+      </c>
+      <c r="E509" s="3">
+        <v>0.84140000000000004</v>
+      </c>
+      <c r="F509" s="3">
+        <v>72</v>
+      </c>
+      <c r="G509" s="2">
+        <v>208</v>
+      </c>
+      <c r="H509" s="3">
+        <v>134</v>
+      </c>
+      <c r="I509" s="3">
+        <v>55</v>
+      </c>
+      <c r="J509" s="3">
+        <v>26</v>
+      </c>
+      <c r="K509" s="2">
+        <v>83</v>
+      </c>
+      <c r="L509" s="3">
+        <v>724</v>
+      </c>
+      <c r="M509" s="2"/>
+    </row>
+    <row r="510" spans="1:13">
+      <c r="A510" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B510" s="2">
+        <v>14</v>
+      </c>
+      <c r="C510" s="2">
+        <v>3</v>
+      </c>
+      <c r="D510" s="3">
+        <v>0.46560000000000001</v>
+      </c>
+      <c r="E510" s="3">
+        <v>0.78920000000000001</v>
+      </c>
+      <c r="F510" s="3">
+        <v>59</v>
+      </c>
+      <c r="G510" s="2">
+        <v>233</v>
+      </c>
+      <c r="H510" s="3">
+        <v>194</v>
+      </c>
+      <c r="I510" s="3">
+        <v>47</v>
+      </c>
+      <c r="J510" s="2">
+        <v>25</v>
+      </c>
+      <c r="K510" s="2">
+        <v>90</v>
+      </c>
+      <c r="L510" s="3">
+        <v>719</v>
+      </c>
+      <c r="M510" s="2"/>
+    </row>
+    <row r="511" spans="1:13">
+      <c r="A511" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B511" s="2">
+        <v>14</v>
+      </c>
+      <c r="C511" s="2">
+        <v>3</v>
+      </c>
+      <c r="D511" s="2">
+        <v>0.45850000000000002</v>
+      </c>
+      <c r="E511" s="2">
+        <v>0.75760000000000005</v>
+      </c>
+      <c r="F511" s="2">
+        <v>56</v>
+      </c>
+      <c r="G511" s="3">
+        <v>248</v>
+      </c>
+      <c r="H511" s="2">
+        <v>159</v>
+      </c>
+      <c r="I511" s="2">
+        <v>43</v>
+      </c>
+      <c r="J511" s="3">
+        <v>38</v>
+      </c>
+      <c r="K511" s="3">
+        <v>86</v>
+      </c>
+      <c r="L511" s="2">
+        <v>670</v>
+      </c>
+      <c r="M511" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -18711,6 +20515,56 @@
     <hyperlink ref="A459" r:id="rId458" tooltip="Ian Banh Mahinmi (Ian Broucek)" display="Ian Banh Mahinmi (28-51-2)"/>
     <hyperlink ref="A460" r:id="rId459" tooltip="No Look No Pass (Josh Dickson)" display="No Look No Pass (43-38)"/>
     <hyperlink ref="A461" r:id="rId460" tooltip="Soccer Karate (Andrew Sarkarati)" display="Soccer Karate (33-48)"/>
+    <hyperlink ref="A462" r:id="rId461" tooltip="Soccer Karate (Andrew Sarkarati)" display="Soccer Karate (50-67)"/>
+    <hyperlink ref="A463" r:id="rId462" tooltip="Delonte's Donuts (Michael Andric)" display="Delonte's Donuts (70-44-3)"/>
+    <hyperlink ref="A464" r:id="rId463" tooltip="What the Blood Clot (Mark Cunningham)" display="What the Blood Clot (65-48-4)"/>
+    <hyperlink ref="A465" r:id="rId464" tooltip="Paul George, John and Ringo (eric broucek)" display="Paul George, John and Ringo (50-67)"/>
+    <hyperlink ref="A466" r:id="rId465" tooltip="Conor's Turpentines (Conor Thompson)" display="Conor's Turpentines (69-42-6)"/>
+    <hyperlink ref="A467" r:id="rId466" tooltip="Ian Banh Mahinmi (Ian Broucek)" display="Ian Banh Mahinmi (42-71-4)"/>
+    <hyperlink ref="A468" r:id="rId467" tooltip="Sami's Mannschaft (sami siegelbaum)" display="Sami's Mannschaft (59-58)"/>
+    <hyperlink ref="A469" r:id="rId468" tooltip="Conquest Pain (Stephen Aldahl)" display="Conquest Pain (54-59-4)"/>
+    <hyperlink ref="A470" r:id="rId469" tooltip="No Look No Pass (Josh Dickson)" display="No Look No Pass (58-59)"/>
+    <hyperlink ref="A471" r:id="rId470" tooltip="Accidental Twitter Hog (Bryce Hesterman)" display="Accidental Twitter Hog (56-58-3)"/>
+    <hyperlink ref="A472" r:id="rId471" tooltip="Delonte's Donuts (Michael Andric)" display="Delonte's Donuts (70-44-3)"/>
+    <hyperlink ref="A473" r:id="rId472" tooltip="Accidental Twitter Hog (Bryce Hesterman)" display="Accidental Twitter Hog (56-58-3)"/>
+    <hyperlink ref="A474" r:id="rId473" tooltip="Soccer Karate (Andrew Sarkarati)" display="Soccer Karate (50-67)"/>
+    <hyperlink ref="A475" r:id="rId474" tooltip="Ian Banh Mahinmi (Ian Broucek)" display="Ian Banh Mahinmi (42-71-4)"/>
+    <hyperlink ref="A476" r:id="rId475" tooltip="Conquest Pain (Stephen Aldahl)" display="Conquest Pain (54-59-4)"/>
+    <hyperlink ref="A477" r:id="rId476" tooltip="Paul George, John and Ringo (eric broucek)" display="Paul George, John and Ringo (50-67)"/>
+    <hyperlink ref="A478" r:id="rId477" tooltip="What the Blood Clot (Mark Cunningham)" display="What the Blood Clot (65-48-4)"/>
+    <hyperlink ref="A479" r:id="rId478" tooltip="No Look No Pass (Josh Dickson)" display="No Look No Pass (58-59)"/>
+    <hyperlink ref="A480" r:id="rId479" tooltip="Sami's Mannschaft (sami siegelbaum)" display="Sami's Mannschaft (59-58)"/>
+    <hyperlink ref="A481" r:id="rId480" tooltip="Conor's Turpentines (Conor Thompson)" display="Conor's Turpentines (69-42-6)"/>
+    <hyperlink ref="A482" r:id="rId481" tooltip="Delonte's Donuts (Michael Andric)" display="Delonte's Donuts (70-44-3)"/>
+    <hyperlink ref="A483" r:id="rId482" tooltip="What the Blood Clot (Mark Cunningham)" display="What the Blood Clot (65-48-4)"/>
+    <hyperlink ref="A484" r:id="rId483" tooltip="No Look No Pass (Josh Dickson)" display="No Look No Pass (58-59)"/>
+    <hyperlink ref="A485" r:id="rId484" tooltip="Conquest Pain (Stephen Aldahl)" display="Conquest Pain (54-59-4)"/>
+    <hyperlink ref="A486" r:id="rId485" tooltip="Ian Banh Mahinmi (Ian Broucek)" display="Ian Banh Mahinmi (42-71-4)"/>
+    <hyperlink ref="A487" r:id="rId486" tooltip="Sami's Mannschaft (sami siegelbaum)" display="Sami's Mannschaft (59-58)"/>
+    <hyperlink ref="A488" r:id="rId487" tooltip="Accidental Twitter Hog (Bryce Hesterman)" display="Accidental Twitter Hog (56-58-3)"/>
+    <hyperlink ref="A489" r:id="rId488" tooltip="Soccer Karate (Andrew Sarkarati)" display="Soccer Karate (50-67)"/>
+    <hyperlink ref="A490" r:id="rId489" tooltip="Paul George, John and Ringo (eric broucek)" display="Paul George, John and Ringo (50-67)"/>
+    <hyperlink ref="A491" r:id="rId490" tooltip="Conor's Turpentines (Conor Thompson)" display="Conor's Turpentines (69-42-6)"/>
+    <hyperlink ref="A492" r:id="rId491" tooltip="No Look No Pass (Josh Dickson)" display="No Look No Pass (58-59)"/>
+    <hyperlink ref="A493" r:id="rId492" tooltip="Delonte's Donuts (Michael Andric)" display="Delonte's Donuts (70-44-3)"/>
+    <hyperlink ref="A494" r:id="rId493" tooltip="Accidental Twitter Hog (Bryce Hesterman)" display="Accidental Twitter Hog (56-58-3)"/>
+    <hyperlink ref="A495" r:id="rId494" tooltip="Sami's Mannschaft (sami siegelbaum)" display="Sami's Mannschaft (59-58)"/>
+    <hyperlink ref="A496" r:id="rId495" tooltip="Conor's Turpentines (Conor Thompson)" display="Conor's Turpentines (69-42-6)"/>
+    <hyperlink ref="A497" r:id="rId496" tooltip="Conquest Pain (Stephen Aldahl)" display="Conquest Pain (54-59-4)"/>
+    <hyperlink ref="A498" r:id="rId497" tooltip="Paul George, John and Ringo (eric broucek)" display="Paul George, John and Ringo (50-67)"/>
+    <hyperlink ref="A499" r:id="rId498" tooltip="Ian Banh Mahinmi (Ian Broucek)" display="Ian Banh Mahinmi (42-71-4)"/>
+    <hyperlink ref="A500" r:id="rId499" tooltip="Soccer Karate (Andrew Sarkarati)" display="Soccer Karate (50-67)"/>
+    <hyperlink ref="A501" r:id="rId500" tooltip="What the Blood Clot (Mark Cunningham)" display="What the Blood Clot (65-48-4)"/>
+    <hyperlink ref="A502" r:id="rId501" tooltip="Paul George, John and Ringo (eric broucek)" display="Paul George, John and Ringo (51-75)"/>
+    <hyperlink ref="A503" r:id="rId502" tooltip="Delonte's Donuts (Michael Andric)" display="Delonte's Donuts (78-45-3)"/>
+    <hyperlink ref="A504" r:id="rId503" tooltip="Ian Banh Mahinmi (Ian Broucek)" display="Ian Banh Mahinmi (46-76-4)"/>
+    <hyperlink ref="A505" r:id="rId504" tooltip="What the Blood Clot (Mark Cunningham)" display="What the Blood Clot (70-52-4)"/>
+    <hyperlink ref="A506" r:id="rId505" tooltip="Conquest Pain (Stephen Aldahl)" display="Conquest Pain (60-62-4)"/>
+    <hyperlink ref="A507" r:id="rId506" tooltip="Soccer Karate (Andrew Sarkarati)" display="Soccer Karate (53-73)"/>
+    <hyperlink ref="A508" r:id="rId507" tooltip="Sami's Mannschaft (sami siegelbaum)" display="Sami's Mannschaft (61-65)"/>
+    <hyperlink ref="A509" r:id="rId508" tooltip="No Look No Pass (Josh Dickson)" display="No Look No Pass (65-61)"/>
+    <hyperlink ref="A510" r:id="rId509" tooltip="Conor's Turpentines (Conor Thompson)" display="Conor's Turpentines (75-45-6)"/>
+    <hyperlink ref="A511" r:id="rId510" tooltip="Accidental Twitter Hog (Bryce Hesterman)" display="Accidental Twitter Hog (59-64-3)"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>